<commit_message>
fixed document. to upload localizations. removed wrong titles.
</commit_message>
<xml_diff>
--- a/Inn_App_Events.xlsx
+++ b/Inn_App_Events.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\GIT\AppleLocalizationUpload\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689AC4A9-02AA-4B66-A5E1-39FA93A5920A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
-  <si>
-    <t>name (30)</t>
-  </si>
-  <si>
-    <t>short (50)</t>
-  </si>
-  <si>
-    <t>long (120)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
   <si>
     <t>locale</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Profondeurs Marines</t>
   </si>
   <si>
-    <t>Plongez, résolvez des puzzles, trouvez l'art caché !</t>
-  </si>
-  <si>
     <t>Terminez des niveaux, collectez des pièces et découvrez de superbes images sous-marines à partager !</t>
   </si>
   <si>
@@ -299,36 +296,55 @@
   </si>
   <si>
     <t>en-CA</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>Plongez, résolvez des puzzles, trouvez l'art c</t>
+  </si>
+  <si>
+    <t>Plongez, résolvepuzzles, trouvez l'art caché !</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -338,7 +354,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -348,7 +364,13 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -362,6 +384,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -370,74 +393,64 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -627,443 +640,448 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.0"/>
-    <col customWidth="1" min="2" max="2" width="39.13"/>
-    <col customWidth="1" min="3" max="3" width="70.5"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
+      <c r="D6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="7" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="B9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="C9" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="6" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="6" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="6" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="6" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D17" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="8" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="7" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="9" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="7" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="B25" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="C25" s="12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="12" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B26" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C26" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="10" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B27" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C27" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="6" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="7" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="14"/>
-      <c r="D30" s="15"/>
-    </row>
-    <row r="32">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="13"/>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>